<commit_message>
company master login tested
</commit_message>
<xml_diff>
--- a/CompanyMaster/src/test/resources/excel/CompanyMaster.xlsx
+++ b/CompanyMaster/src/test/resources/excel/CompanyMaster.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\deepak\New-office\code\Eclipse-workspace\selenium\CompanyMaster\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066F1BD7-D5AC-4B3D-917D-597256A58947}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE88FE05-A9CB-4ACD-A8EB-CFC8A266F3B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{B5040D02-B1ED-408E-9851-00438E4076DF}"/>
+    <workbookView xWindow="2055" yWindow="4155" windowWidth="14400" windowHeight="10755" activeTab="2" xr2:uid="{B5040D02-B1ED-408E-9851-00438E4076DF}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="LoginTest" sheetId="2" r:id="rId2"/>
+    <sheet name="AddCompany" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Password</t>
   </si>
@@ -85,13 +86,40 @@
     <t>id</t>
   </si>
   <si>
-    <t>_com_liferay_login_web_portlet_LoginPortlet_wkmi</t>
-  </si>
-  <si>
     <t>_com_liferay_login_web_portlet_LoginPortlet_password</t>
   </si>
   <si>
     <t>john.smith</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>lfr-btn-label</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>john.smith1</t>
+  </si>
+  <si>
+    <t>askd</t>
+  </si>
+  <si>
+    <t>Global Files</t>
+  </si>
+  <si>
+    <t>Company Master</t>
+  </si>
+  <si>
+    <t>//*[contains(text(), ' Global Files ')]</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Company Master')]</t>
   </si>
 </sst>
 </file>
@@ -471,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A648334-2125-4C79-B696-79270EF66D95}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,10 +523,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +558,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,14 +629,129 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F76510B-15FA-4763-B404-5847360608AF}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added plugin for xml runing throug maven
</commit_message>
<xml_diff>
--- a/CompanyMaster/src/test/resources/excel/CompanyMaster.xlsx
+++ b/CompanyMaster/src/test/resources/excel/CompanyMaster.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\deepak\New-office\code\Eclipse-workspace\selenium\CompanyMaster\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepak\Desktop\Git\Selenium\Selenium\CompanyMaster\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE88FE05-A9CB-4ACD-A8EB-CFC8A266F3B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="4155" windowWidth="14400" windowHeight="10755" activeTab="2" xr2:uid="{B5040D02-B1ED-408E-9851-00438E4076DF}"/>
+    <workbookView xWindow="2055" yWindow="4155" windowWidth="14400" windowHeight="10755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="LoginTest" sheetId="2" r:id="rId2"/>
     <sheet name="AddCompany" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Password</t>
   </si>
@@ -120,13 +119,43 @@
   </si>
   <si>
     <t>//span[contains(text(),'Company Master')]</t>
+  </si>
+  <si>
+    <t>gtnAddButton</t>
+  </si>
+  <si>
+    <t>companyAdd</t>
+  </si>
+  <si>
+    <t>companyInformation</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Company Information')]</t>
+  </si>
+  <si>
+    <t>companyInformationTabCompanyId</t>
+  </si>
+  <si>
+    <t>companyId</t>
+  </si>
+  <si>
+    <t>companyInformationTabCompanyNo</t>
+  </si>
+  <si>
+    <t>companyNo</t>
+  </si>
+  <si>
+    <t>companyInformationTabCompanyName</t>
+  </si>
+  <si>
+    <t>companyName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +186,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,11 +214,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -498,7 +534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A648334-2125-4C79-B696-79270EF66D95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -547,14 +583,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="john.smith@sysbiz.com" xr:uid="{E179E3BC-378E-4E2F-BD35-0B078CCE9CE4}"/>
+    <hyperlink ref="A2" r:id="rId1" display="john.smith@sysbiz.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B217-3094-4245-A4DB-6124A8192307}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -642,11 +678,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F76510B-15FA-4763-B404-5847360608AF}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +787,78 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
popup combobox test added
</commit_message>
<xml_diff>
--- a/CompanyMaster/src/test/resources/excel/CompanyMaster.xlsx
+++ b/CompanyMaster/src/test/resources/excel/CompanyMaster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\deepak\New-office\git-code\Selenium\Selenium\CompanyMaster\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B6E2BB-179B-403B-AD18-17F175FCCD08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF3F8C4-72B1-41F4-80FF-AB50E7BBB3C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="159">
   <si>
     <t>Password</t>
   </si>
@@ -1109,13 +1109,130 @@
   </si>
   <si>
     <t>IdentifierAttach</t>
+  </si>
+  <si>
+    <t>gwt-uid-86</t>
+  </si>
+  <si>
+    <t>CompanyTradeClassTab</t>
+  </si>
+  <si>
+    <t>Chargeback</t>
+  </si>
+  <si>
+    <t>TradeClass</t>
+  </si>
+  <si>
+    <t>10/10/2019'</t>
+  </si>
+  <si>
+    <t>12/10/2019'</t>
+  </si>
+  <si>
+    <t>TradeClassStartDate</t>
+  </si>
+  <si>
+    <t>TradeClassEndDate</t>
+  </si>
+  <si>
+    <t>tradeClassAttachButton</t>
+  </si>
+  <si>
+    <t>TradeClassAttachButton</t>
+  </si>
+  <si>
+    <t>gwt-uid-123</t>
+  </si>
+  <si>
+    <t>gwt-uid-125</t>
+  </si>
+  <si>
+    <t>gwt-uid-127</t>
+  </si>
+  <si>
+    <t>gwt-uid-87</t>
+  </si>
+  <si>
+    <t>parentCompanyNo</t>
+  </si>
+  <si>
+    <t>PArentCompanyNo</t>
+  </si>
+  <si>
+    <t>ParentCompanyTab</t>
+  </si>
+  <si>
+    <t>parentCompanySearchcompanyId</t>
+  </si>
+  <si>
+    <t>CompanyIDSearch</t>
+  </si>
+  <si>
+    <t>parentCompanySearchcompanyNo</t>
+  </si>
+  <si>
+    <t>BPI*</t>
+  </si>
+  <si>
+    <t>B*</t>
+  </si>
+  <si>
+    <t>comapnyNoSearch</t>
+  </si>
+  <si>
+    <t>Cigna*</t>
+  </si>
+  <si>
+    <t>CompanyNoSearch</t>
+  </si>
+  <si>
+    <t>parentCompanySearchcompanyName</t>
+  </si>
+  <si>
+    <t>CompanyStatusSearch</t>
+  </si>
+  <si>
+    <t>searchtableRow</t>
+  </si>
+  <si>
+    <t>parentCompanySelectButton</t>
+  </si>
+  <si>
+    <t>MCO</t>
+  </si>
+  <si>
+    <t>ComapnyTypeSearch</t>
+  </si>
+  <si>
+    <t>parentCompanygtnSearch01</t>
+  </si>
+  <si>
+    <t>SearchButtonParentCompany</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>//*[@id="parentCompanySearchcompanyStatus"]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="parentCompanySearchcompanyType"]/input</t>
+  </si>
+  <si>
+    <t>(//tr[@class='v-table-row'])[1]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1188,6 +1305,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1210,7 +1333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1223,6 +1346,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1682,658 +1806,1054 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" customWidth="1"/>
+    <col min="1" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>79</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
       <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
       <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
       <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>42</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>42</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" t="s">
         <v>73</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" t="s">
         <v>74</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>42</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>42</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>42</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" t="s">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" t="s">
         <v>84</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>13</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" t="s">
         <v>84</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" t="s">
         <v>91</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
         <v>94</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>13</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
         <v>96</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>42</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" t="s">
         <v>106</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" t="s">
         <v>108</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>13</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>42</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>48</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>48</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C39" t="s">
+      <c r="B39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>